<commit_message>
Changes database to postgresSQL
</commit_message>
<xml_diff>
--- a/lib/menu.xlsx
+++ b/lib/menu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Shadow Cakes App\webapp\shadowCakes\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBCBC11-B8DA-4412-844D-F760DB36D45A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D5A1E5-4D53-4323-8476-576500CACFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5140" windowWidth="38620" windowHeight="21220" tabRatio="926" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="926" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="14" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="359">
   <si>
     <t xml:space="preserve">vanilla </t>
   </si>
@@ -1162,19 +1162,19 @@
     <t>category_id</t>
   </si>
   <si>
-    <t>Sizes</t>
-  </si>
-  <si>
-    <t>Feeds</t>
-  </si>
-  <si>
-    <t>6 in, 8 in</t>
-  </si>
-  <si>
-    <t>6 inches feeds 5…..</t>
-  </si>
-  <si>
-    <t>Added Cost</t>
+    <t>mult_size</t>
+  </si>
+  <si>
+    <t>sizes</t>
+  </si>
+  <si>
+    <t>{6 in, 8in}</t>
+  </si>
+  <si>
+    <t>{15, 10}</t>
+  </si>
+  <si>
+    <t>priceDiff</t>
   </si>
 </sst>
 </file>
@@ -2196,6 +2196,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2253,6 +2256,48 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="55" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="55" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="55" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="33" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="33" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
@@ -2306,51 +2351,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="55" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="55" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="55" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="33" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="33" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="129">
@@ -2553,14 +2553,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2570,7 +2570,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2639,14 +2639,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2656,7 +2656,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2730,14 +2730,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2747,7 +2747,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3089,8 +3089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3409478-BB8A-4EB4-ACC6-5CDC2C1DB2F9}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3176,14 +3176,14 @@
       <c r="J2" s="149" t="s">
         <v>344</v>
       </c>
-      <c r="K2" s="201" t="s">
+      <c r="K2" s="150" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="L2" s="149" t="s">
+      <c r="M2" s="149" t="s">
         <v>357</v>
-      </c>
-      <c r="M2" s="149">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3217,6 +3217,15 @@
       <c r="J3" s="149" t="s">
         <v>338</v>
       </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="149" t="s">
+        <v>356</v>
+      </c>
+      <c r="M3" s="149" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -3247,6 +3256,9 @@
         <v>0</v>
       </c>
       <c r="J4" s="149"/>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="149" t="s">
@@ -3278,6 +3290,15 @@
       </c>
       <c r="J5" s="149" t="s">
         <v>343</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="149" t="s">
+        <v>356</v>
+      </c>
+      <c r="M5" s="149" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3321,21 +3342,21 @@
     </row>
     <row r="4" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="151" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
-      <c r="E5" s="151"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="151"/>
-      <c r="H5" s="151"/>
-      <c r="I5" s="151"/>
-      <c r="J5" s="151"/>
-      <c r="K5" s="151"/>
-      <c r="L5" s="151"/>
-      <c r="M5" s="151"/>
-      <c r="N5" s="152"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
+      <c r="J5" s="152"/>
+      <c r="K5" s="152"/>
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="153"/>
     </row>
     <row r="6" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
@@ -4421,10 +4442,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>239</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -4443,8 +4464,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="155"/>
-      <c r="B3" s="153"/>
+      <c r="A3" s="156"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="11" t="s">
         <v>52</v>
       </c>
@@ -4461,8 +4482,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
-      <c r="B4" s="153"/>
+      <c r="A4" s="156"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="11" t="s">
         <v>64</v>
       </c>
@@ -4479,8 +4500,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
-      <c r="B5" s="153"/>
+      <c r="A5" s="156"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="11" t="s">
         <v>53</v>
       </c>
@@ -4497,8 +4518,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
-      <c r="B6" s="153"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="11" t="s">
         <v>54</v>
       </c>
@@ -4515,8 +4536,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="B7" s="153"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="154"/>
       <c r="C7" s="11" t="s">
         <v>55</v>
       </c>
@@ -4533,8 +4554,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="153"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="11" t="s">
         <v>56</v>
       </c>
@@ -4551,8 +4572,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
-      <c r="B9" s="153"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="154"/>
       <c r="C9" s="11" t="s">
         <v>57</v>
       </c>
@@ -4569,8 +4590,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
-      <c r="B10" s="153"/>
+      <c r="A10" s="156"/>
+      <c r="B10" s="154"/>
       <c r="C10" s="11" t="s">
         <v>68</v>
       </c>
@@ -4587,8 +4608,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="155"/>
-      <c r="B11" s="153"/>
+      <c r="A11" s="156"/>
+      <c r="B11" s="154"/>
       <c r="C11" s="11" t="s">
         <v>58</v>
       </c>
@@ -4605,8 +4626,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="155"/>
-      <c r="B12" s="153"/>
+      <c r="A12" s="156"/>
+      <c r="B12" s="154"/>
       <c r="C12" s="11" t="s">
         <v>59</v>
       </c>
@@ -4627,32 +4648,32 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
+      <c r="A13" s="156"/>
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
+      <c r="A14" s="156"/>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
+      <c r="A15" s="156"/>
       <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
+      <c r="A16" s="156"/>
       <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
-      <c r="B17" s="154" t="s">
+      <c r="A17" s="156"/>
+      <c r="B17" s="155" t="s">
         <v>240</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -4671,8 +4692,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
-      <c r="B18" s="154"/>
+      <c r="A18" s="156"/>
+      <c r="B18" s="155"/>
       <c r="C18" s="16" t="s">
         <v>52</v>
       </c>
@@ -4689,8 +4710,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
-      <c r="B19" s="154"/>
+      <c r="A19" s="156"/>
+      <c r="B19" s="155"/>
       <c r="C19" s="16" t="s">
         <v>64</v>
       </c>
@@ -4707,8 +4728,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
-      <c r="B20" s="154"/>
+      <c r="A20" s="156"/>
+      <c r="B20" s="155"/>
       <c r="C20" s="16" t="s">
         <v>53</v>
       </c>
@@ -4725,8 +4746,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
-      <c r="B21" s="154"/>
+      <c r="A21" s="156"/>
+      <c r="B21" s="155"/>
       <c r="C21" s="16" t="s">
         <v>54</v>
       </c>
@@ -4743,8 +4764,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
-      <c r="B22" s="154"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="155"/>
       <c r="C22" s="16" t="s">
         <v>55</v>
       </c>
@@ -4761,8 +4782,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
-      <c r="B23" s="154"/>
+      <c r="A23" s="156"/>
+      <c r="B23" s="155"/>
       <c r="C23" s="16" t="s">
         <v>56</v>
       </c>
@@ -4783,8 +4804,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
-      <c r="B24" s="154"/>
+      <c r="A24" s="156"/>
+      <c r="B24" s="155"/>
       <c r="C24" s="16" t="s">
         <v>57</v>
       </c>
@@ -4801,8 +4822,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
-      <c r="B25" s="154"/>
+      <c r="A25" s="156"/>
+      <c r="B25" s="155"/>
       <c r="C25" s="16" t="s">
         <v>67</v>
       </c>
@@ -4819,8 +4840,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="155"/>
-      <c r="B26" s="154"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="155"/>
       <c r="C26" s="16" t="s">
         <v>58</v>
       </c>
@@ -4836,8 +4857,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
-      <c r="B27" s="154"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="155"/>
       <c r="C27" s="16" t="s">
         <v>59</v>
       </c>
@@ -4854,8 +4875,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="155"/>
-      <c r="B28" s="154"/>
+      <c r="A28" s="156"/>
+      <c r="B28" s="155"/>
       <c r="C28" s="16" t="s">
         <v>65</v>
       </c>
@@ -4873,8 +4894,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="155"/>
-      <c r="B29" s="154"/>
+      <c r="A29" s="156"/>
+      <c r="B29" s="155"/>
       <c r="C29" s="16" t="s">
         <v>66</v>
       </c>
@@ -4895,31 +4916,31 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="155"/>
+      <c r="A30" s="156"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="155"/>
+      <c r="A31" s="156"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="155"/>
+      <c r="A32" s="156"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="155"/>
+      <c r="A33" s="156"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="155"/>
+      <c r="A34" s="156"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="155"/>
+      <c r="A35" s="156"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="155"/>
+      <c r="A36" s="156"/>
     </row>
     <row r="37" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="155"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4928,111 +4949,111 @@
       <c r="G37" s="61"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="155"/>
+      <c r="A38" s="156"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="155"/>
+      <c r="A39" s="156"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="155"/>
+      <c r="A40" s="156"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="155"/>
+      <c r="A41" s="156"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="155"/>
+      <c r="A42" s="156"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="155"/>
+      <c r="A43" s="156"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="155"/>
+      <c r="A44" s="156"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="155"/>
+      <c r="A45" s="156"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="155"/>
+      <c r="A46" s="156"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="155"/>
+      <c r="A47" s="156"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="155"/>
+      <c r="A48" s="156"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="155"/>
+      <c r="A49" s="156"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="155"/>
+      <c r="A50" s="156"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="155"/>
+      <c r="A51" s="156"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="155"/>
+      <c r="A52" s="156"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="155"/>
+      <c r="A53" s="156"/>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="155"/>
+      <c r="A54" s="156"/>
       <c r="B54" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="155"/>
+      <c r="A55" s="156"/>
       <c r="B55" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="155"/>
+      <c r="A56" s="156"/>
       <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="155"/>
+      <c r="A57" s="156"/>
       <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="155"/>
+      <c r="A58" s="156"/>
       <c r="B58" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="155"/>
+      <c r="A59" s="156"/>
       <c r="B59" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="155"/>
+      <c r="A60" s="156"/>
       <c r="B60" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="155"/>
+      <c r="A61" s="156"/>
       <c r="B61" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="155"/>
+      <c r="A62" s="156"/>
       <c r="B62" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="155"/>
+      <c r="A63" s="156"/>
       <c r="B63" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="155"/>
+      <c r="A64" s="156"/>
       <c r="B64" s="3" t="s">
         <v>15</v>
       </c>
@@ -5072,7 +5093,7 @@
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
-      <c r="B71" s="156" t="s">
+      <c r="B71" s="157" t="s">
         <v>244</v>
       </c>
       <c r="C71" s="17" t="s">
@@ -5092,7 +5113,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
-      <c r="B72" s="157"/>
+      <c r="B72" s="158"/>
       <c r="C72" s="17" t="s">
         <v>76</v>
       </c>
@@ -5110,7 +5131,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
-      <c r="B73" s="157"/>
+      <c r="B73" s="158"/>
       <c r="C73" s="17" t="s">
         <v>77</v>
       </c>
@@ -5128,7 +5149,7 @@
     </row>
     <row r="74" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
-      <c r="B74" s="157"/>
+      <c r="B74" s="158"/>
       <c r="C74" s="17" t="s">
         <v>55</v>
       </c>
@@ -5146,7 +5167,7 @@
     </row>
     <row r="75" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
-      <c r="B75" s="158"/>
+      <c r="B75" s="159"/>
       <c r="C75" s="17" t="s">
         <v>59</v>
       </c>
@@ -5175,7 +5196,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
-      <c r="B77" s="159" t="s">
+      <c r="B77" s="160" t="s">
         <v>243</v>
       </c>
       <c r="C77" s="26" t="s">
@@ -5196,7 +5217,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
-      <c r="B78" s="159"/>
+      <c r="B78" s="160"/>
       <c r="C78" s="26" t="s">
         <v>76</v>
       </c>
@@ -5215,7 +5236,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
-      <c r="B79" s="159"/>
+      <c r="B79" s="160"/>
       <c r="C79" s="26" t="s">
         <v>78</v>
       </c>
@@ -5234,7 +5255,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
-      <c r="B80" s="159"/>
+      <c r="B80" s="160"/>
       <c r="C80" s="26" t="s">
         <v>79</v>
       </c>
@@ -5253,7 +5274,7 @@
     </row>
     <row r="81" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
-      <c r="B81" s="159"/>
+      <c r="B81" s="160"/>
       <c r="C81" s="26" t="s">
         <v>80</v>
       </c>
@@ -5272,7 +5293,7 @@
     </row>
     <row r="82" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
-      <c r="B82" s="159"/>
+      <c r="B82" s="160"/>
       <c r="C82" s="26" t="s">
         <v>59</v>
       </c>
@@ -6921,7 +6942,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="157" t="s">
         <v>242</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -6941,7 +6962,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="157"/>
+      <c r="A3" s="158"/>
       <c r="B3" s="17" t="s">
         <v>76</v>
       </c>
@@ -6959,7 +6980,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="157"/>
+      <c r="A4" s="158"/>
       <c r="B4" s="17" t="s">
         <v>77</v>
       </c>
@@ -6977,7 +6998,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="157"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="17" t="s">
         <v>55</v>
       </c>
@@ -6995,7 +7016,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="158"/>
+      <c r="A6" s="159"/>
       <c r="B6" s="17" t="s">
         <v>59</v>
       </c>
@@ -7019,7 +7040,7 @@
       <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="160" t="s">
         <v>288</v>
       </c>
       <c r="B8" s="26" t="s">
@@ -7039,7 +7060,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="159"/>
+      <c r="A9" s="160"/>
       <c r="B9" s="26" t="s">
         <v>76</v>
       </c>
@@ -7057,7 +7078,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="159"/>
+      <c r="A10" s="160"/>
       <c r="B10" s="26" t="s">
         <v>64</v>
       </c>
@@ -7075,7 +7096,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="159"/>
+      <c r="A11" s="160"/>
       <c r="B11" s="26" t="s">
         <v>289</v>
       </c>
@@ -7093,7 +7114,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="159"/>
+      <c r="A12" s="160"/>
       <c r="B12" s="97" t="s">
         <v>80</v>
       </c>
@@ -7110,7 +7131,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="159"/>
+      <c r="A13" s="160"/>
       <c r="B13" s="26" t="s">
         <v>59</v>
       </c>
@@ -7131,7 +7152,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="165" t="s">
+      <c r="A15" s="166" t="s">
         <v>301</v>
       </c>
       <c r="B15" s="98" t="s">
@@ -7151,7 +7172,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="165"/>
+      <c r="A16" s="166"/>
       <c r="B16" s="98" t="s">
         <v>76</v>
       </c>
@@ -7169,7 +7190,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="165"/>
+      <c r="A17" s="166"/>
       <c r="B17" s="98" t="s">
         <v>64</v>
       </c>
@@ -7187,7 +7208,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="165"/>
+      <c r="A18" s="166"/>
       <c r="B18" s="98" t="s">
         <v>289</v>
       </c>
@@ -7205,7 +7226,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="165"/>
+      <c r="A19" s="166"/>
       <c r="B19" s="101" t="s">
         <v>80</v>
       </c>
@@ -7222,7 +7243,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="165"/>
+      <c r="A20" s="166"/>
       <c r="B20" s="98" t="s">
         <v>59</v>
       </c>
@@ -7251,7 +7272,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="160" t="s">
+      <c r="A22" s="161" t="s">
         <v>294</v>
       </c>
       <c r="B22" s="110" t="s">
@@ -7271,7 +7292,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="161"/>
+      <c r="A23" s="162"/>
       <c r="B23" s="110" t="s">
         <v>290</v>
       </c>
@@ -7289,7 +7310,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="161"/>
+      <c r="A24" s="162"/>
       <c r="B24" s="110" t="s">
         <v>292</v>
       </c>
@@ -7307,7 +7328,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="161"/>
+      <c r="A25" s="162"/>
       <c r="B25" s="110" t="s">
         <v>291</v>
       </c>
@@ -7325,7 +7346,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="161"/>
+      <c r="A26" s="162"/>
       <c r="B26" s="113" t="s">
         <v>293</v>
       </c>
@@ -7341,7 +7362,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="162"/>
+      <c r="A27" s="163"/>
       <c r="B27" s="110" t="s">
         <v>59</v>
       </c>
@@ -7362,7 +7383,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="163" t="s">
+      <c r="A29" s="164" t="s">
         <v>295</v>
       </c>
       <c r="B29" s="105" t="s">
@@ -7382,7 +7403,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="163"/>
+      <c r="A30" s="164"/>
       <c r="B30" s="105" t="s">
         <v>292</v>
       </c>
@@ -7400,7 +7421,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="163"/>
+      <c r="A31" s="164"/>
       <c r="B31" s="105" t="s">
         <v>291</v>
       </c>
@@ -7418,7 +7439,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="163"/>
+      <c r="A32" s="164"/>
       <c r="B32" s="105" t="s">
         <v>289</v>
       </c>
@@ -7436,7 +7457,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="163"/>
+      <c r="A33" s="164"/>
       <c r="B33" s="108"/>
       <c r="C33" s="105">
         <v>0</v>
@@ -7450,7 +7471,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="163"/>
+      <c r="A34" s="164"/>
       <c r="B34" s="105" t="s">
         <v>59</v>
       </c>
@@ -7471,7 +7492,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="165" t="s">
         <v>296</v>
       </c>
       <c r="B36" s="57" t="s">
@@ -7491,7 +7512,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="164"/>
+      <c r="A37" s="165"/>
       <c r="B37" s="57" t="s">
         <v>299</v>
       </c>
@@ -7509,7 +7530,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="164"/>
+      <c r="A38" s="165"/>
       <c r="B38" s="57" t="s">
         <v>300</v>
       </c>
@@ -7527,7 +7548,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="164"/>
+      <c r="A39" s="165"/>
       <c r="B39" s="57" t="s">
         <v>55</v>
       </c>
@@ -7545,7 +7566,7 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="164"/>
+      <c r="A40" s="165"/>
       <c r="B40" s="103">
         <v>0</v>
       </c>
@@ -7561,7 +7582,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="164"/>
+      <c r="A41" s="165"/>
       <c r="B41" s="57" t="s">
         <v>59</v>
       </c>
@@ -7617,7 +7638,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="167" t="s">
         <v>274</v>
       </c>
       <c r="C2" s="67" t="s">
@@ -7637,7 +7658,7 @@
       <c r="G2" s="71"/>
     </row>
     <row r="3" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="167"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="67" t="s">
         <v>54</v>
       </c>
@@ -7655,7 +7676,7 @@
       <c r="G3" s="71"/>
     </row>
     <row r="4" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="167"/>
+      <c r="B4" s="168"/>
       <c r="C4" s="67" t="s">
         <v>265</v>
       </c>
@@ -7673,7 +7694,7 @@
       <c r="G4" s="71"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="167"/>
+      <c r="B5" s="168"/>
       <c r="C5" s="67" t="s">
         <v>266</v>
       </c>
@@ -7691,7 +7712,7 @@
       <c r="G5" s="71"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="167"/>
+      <c r="B6" s="168"/>
       <c r="C6" s="67" t="s">
         <v>53</v>
       </c>
@@ -7709,7 +7730,7 @@
       <c r="G6" s="71"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="167"/>
+      <c r="B7" s="168"/>
       <c r="C7" s="67" t="s">
         <v>63</v>
       </c>
@@ -7727,7 +7748,7 @@
       <c r="G7" s="71"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="167"/>
+      <c r="B8" s="168"/>
       <c r="C8" s="67" t="s">
         <v>55</v>
       </c>
@@ -7745,7 +7766,7 @@
       <c r="G8" s="71"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="167"/>
+      <c r="B9" s="168"/>
       <c r="C9" s="67" t="s">
         <v>267</v>
       </c>
@@ -7763,7 +7784,7 @@
       <c r="G9" s="71"/>
     </row>
     <row r="10" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="167"/>
+      <c r="B10" s="168"/>
       <c r="C10" s="67" t="s">
         <v>268</v>
       </c>
@@ -7781,7 +7802,7 @@
       <c r="G10" s="71"/>
     </row>
     <row r="11" spans="2:7" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="167"/>
+      <c r="B11" s="168"/>
       <c r="C11" s="67" t="s">
         <v>269</v>
       </c>
@@ -7799,7 +7820,7 @@
       <c r="G11" s="71"/>
     </row>
     <row r="12" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="168"/>
+      <c r="B12" s="169"/>
       <c r="C12" s="68" t="s">
         <v>59</v>
       </c>
@@ -7820,7 +7841,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="166" t="s">
+      <c r="B14" s="167" t="s">
         <v>282</v>
       </c>
       <c r="C14" s="67" t="s">
@@ -7840,7 +7861,7 @@
       <c r="G14" s="71"/>
     </row>
     <row r="15" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="167"/>
+      <c r="B15" s="168"/>
       <c r="C15" s="67" t="s">
         <v>54</v>
       </c>
@@ -7858,7 +7879,7 @@
       <c r="G15" s="71"/>
     </row>
     <row r="16" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="167"/>
+      <c r="B16" s="168"/>
       <c r="C16" s="67" t="s">
         <v>265</v>
       </c>
@@ -7876,7 +7897,7 @@
       <c r="G16" s="71"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="167"/>
+      <c r="B17" s="168"/>
       <c r="C17" s="67" t="s">
         <v>266</v>
       </c>
@@ -7894,7 +7915,7 @@
       <c r="G17" s="71"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="167"/>
+      <c r="B18" s="168"/>
       <c r="C18" s="67" t="s">
         <v>53</v>
       </c>
@@ -7912,7 +7933,7 @@
       <c r="G18" s="71"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="167"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="67" t="s">
         <v>63</v>
       </c>
@@ -7930,7 +7951,7 @@
       <c r="G19" s="71"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="167"/>
+      <c r="B20" s="168"/>
       <c r="C20" s="67" t="s">
         <v>55</v>
       </c>
@@ -7948,7 +7969,7 @@
       <c r="G20" s="71"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="167"/>
+      <c r="B21" s="168"/>
       <c r="C21" s="67" t="s">
         <v>267</v>
       </c>
@@ -7966,7 +7987,7 @@
       <c r="G21" s="71"/>
     </row>
     <row r="22" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="167"/>
+      <c r="B22" s="168"/>
       <c r="C22" s="67" t="s">
         <v>268</v>
       </c>
@@ -7984,7 +8005,7 @@
       <c r="G22" s="71"/>
     </row>
     <row r="23" spans="2:7" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="167"/>
+      <c r="B23" s="168"/>
       <c r="C23" s="67" t="s">
         <v>269</v>
       </c>
@@ -8002,7 +8023,7 @@
       <c r="G23" s="71"/>
     </row>
     <row r="24" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="168"/>
+      <c r="B24" s="169"/>
       <c r="C24" s="67" t="s">
         <v>283</v>
       </c>
@@ -8085,7 +8106,7 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="172" t="s">
+      <c r="A3" s="187" t="s">
         <v>239</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -8104,7 +8125,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="173"/>
+      <c r="A4" s="188"/>
       <c r="B4" s="11" t="s">
         <v>52</v>
       </c>
@@ -8121,7 +8142,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="173"/>
+      <c r="A5" s="188"/>
       <c r="B5" s="11" t="s">
         <v>64</v>
       </c>
@@ -8138,7 +8159,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="173"/>
+      <c r="A6" s="188"/>
       <c r="B6" s="11" t="s">
         <v>53</v>
       </c>
@@ -8155,7 +8176,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="173"/>
+      <c r="A7" s="188"/>
       <c r="B7" s="11" t="s">
         <v>54</v>
       </c>
@@ -8172,7 +8193,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="173"/>
+      <c r="A8" s="188"/>
       <c r="B8" s="11" t="s">
         <v>55</v>
       </c>
@@ -8189,7 +8210,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="173"/>
+      <c r="A9" s="188"/>
       <c r="B9" s="11" t="s">
         <v>56</v>
       </c>
@@ -8206,7 +8227,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="173"/>
+      <c r="A10" s="188"/>
       <c r="B10" s="11" t="s">
         <v>57</v>
       </c>
@@ -8223,7 +8244,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="173"/>
+      <c r="A11" s="188"/>
       <c r="B11" s="11" t="s">
         <v>68</v>
       </c>
@@ -8240,7 +8261,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="173"/>
+      <c r="A12" s="188"/>
       <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
@@ -8257,7 +8278,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="174"/>
+      <c r="A13" s="189"/>
       <c r="B13" s="11" t="s">
         <v>59</v>
       </c>
@@ -8278,7 +8299,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="175" t="s">
+      <c r="A15" s="190" t="s">
         <v>264</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -8297,7 +8318,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="176"/>
+      <c r="A16" s="191"/>
       <c r="B16" s="16" t="s">
         <v>52</v>
       </c>
@@ -8314,7 +8335,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="176"/>
+      <c r="A17" s="191"/>
       <c r="B17" s="16" t="s">
         <v>64</v>
       </c>
@@ -8331,7 +8352,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="176"/>
+      <c r="A18" s="191"/>
       <c r="B18" s="16" t="s">
         <v>53</v>
       </c>
@@ -8348,7 +8369,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="176"/>
+      <c r="A19" s="191"/>
       <c r="B19" s="16" t="s">
         <v>54</v>
       </c>
@@ -8365,7 +8386,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="176"/>
+      <c r="A20" s="191"/>
       <c r="B20" s="16" t="s">
         <v>55</v>
       </c>
@@ -8382,7 +8403,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="176"/>
+      <c r="A21" s="191"/>
       <c r="B21" s="16" t="s">
         <v>56</v>
       </c>
@@ -8399,7 +8420,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="176"/>
+      <c r="A22" s="191"/>
       <c r="B22" s="16" t="s">
         <v>57</v>
       </c>
@@ -8416,7 +8437,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="176"/>
+      <c r="A23" s="191"/>
       <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
@@ -8433,7 +8454,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="176"/>
+      <c r="A24" s="191"/>
       <c r="B24" s="16" t="s">
         <v>58</v>
       </c>
@@ -8450,7 +8471,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="176"/>
+      <c r="A25" s="191"/>
       <c r="B25" s="16" t="s">
         <v>59</v>
       </c>
@@ -8467,7 +8488,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="176"/>
+      <c r="A26" s="191"/>
       <c r="B26" s="16" t="s">
         <v>65</v>
       </c>
@@ -8485,7 +8506,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="177"/>
+      <c r="A27" s="192"/>
       <c r="B27" s="16" t="s">
         <v>66</v>
       </c>
@@ -8505,7 +8526,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="178" t="s">
+      <c r="A29" s="193" t="s">
         <v>245</v>
       </c>
       <c r="B29" s="51" t="s">
@@ -8525,7 +8546,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="179"/>
+      <c r="A30" s="194"/>
       <c r="B30" s="51" t="s">
         <v>246</v>
       </c>
@@ -8543,7 +8564,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="179"/>
+      <c r="A31" s="194"/>
       <c r="B31" s="51" t="s">
         <v>247</v>
       </c>
@@ -8561,7 +8582,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="179"/>
+      <c r="A32" s="194"/>
       <c r="B32" s="51" t="s">
         <v>56</v>
       </c>
@@ -8579,7 +8600,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="179"/>
+      <c r="A33" s="194"/>
       <c r="B33" s="51" t="s">
         <v>248</v>
       </c>
@@ -8597,7 +8618,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="180"/>
+      <c r="A34" s="195"/>
       <c r="B34" s="52" t="s">
         <v>249</v>
       </c>
@@ -8618,7 +8639,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="181" t="s">
+      <c r="A36" s="196" t="s">
         <v>253</v>
       </c>
       <c r="B36" s="56" t="s">
@@ -8638,7 +8659,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="182"/>
+      <c r="A37" s="197"/>
       <c r="B37" s="56" t="s">
         <v>246</v>
       </c>
@@ -8656,7 +8677,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="182"/>
+      <c r="A38" s="197"/>
       <c r="B38" s="56" t="s">
         <v>247</v>
       </c>
@@ -8674,7 +8695,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="182"/>
+      <c r="A39" s="197"/>
       <c r="B39" s="56" t="s">
         <v>56</v>
       </c>
@@ -8692,7 +8713,7 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="182"/>
+      <c r="A40" s="197"/>
       <c r="B40" s="56" t="s">
         <v>248</v>
       </c>
@@ -8710,7 +8731,7 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="182"/>
+      <c r="A41" s="197"/>
       <c r="B41" s="56" t="s">
         <v>252</v>
       </c>
@@ -8728,7 +8749,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="183"/>
+      <c r="A42" s="198"/>
       <c r="B42" s="57" t="s">
         <v>249</v>
       </c>
@@ -8749,7 +8770,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="184" t="s">
+      <c r="A44" s="199" t="s">
         <v>255</v>
       </c>
       <c r="B44" s="64" t="s">
@@ -8769,7 +8790,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="185"/>
+      <c r="A45" s="200"/>
       <c r="B45" s="64" t="s">
         <v>246</v>
       </c>
@@ -8787,7 +8808,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="185"/>
+      <c r="A46" s="200"/>
       <c r="B46" s="64" t="s">
         <v>254</v>
       </c>
@@ -8805,7 +8826,7 @@
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="185"/>
+      <c r="A47" s="200"/>
       <c r="B47" s="64" t="s">
         <v>56</v>
       </c>
@@ -8823,7 +8844,7 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="185"/>
+      <c r="A48" s="200"/>
       <c r="B48" s="64" t="s">
         <v>248</v>
       </c>
@@ -8841,7 +8862,7 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="186"/>
+      <c r="A49" s="201"/>
       <c r="B49" s="26" t="s">
         <v>249</v>
       </c>
@@ -8862,7 +8883,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="169" t="s">
+      <c r="A51" s="184" t="s">
         <v>260</v>
       </c>
       <c r="B51" s="51" t="s">
@@ -8882,7 +8903,7 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="170"/>
+      <c r="A52" s="185"/>
       <c r="B52" s="51" t="s">
         <v>246</v>
       </c>
@@ -8900,7 +8921,7 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="170"/>
+      <c r="A53" s="185"/>
       <c r="B53" s="51" t="s">
         <v>262</v>
       </c>
@@ -8918,7 +8939,7 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="170"/>
+      <c r="A54" s="185"/>
       <c r="B54" s="51" t="s">
         <v>56</v>
       </c>
@@ -8936,7 +8957,7 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="170"/>
+      <c r="A55" s="185"/>
       <c r="B55" s="51" t="s">
         <v>75</v>
       </c>
@@ -8954,7 +8975,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="170"/>
+      <c r="A56" s="185"/>
       <c r="B56" s="51" t="s">
         <v>58</v>
       </c>
@@ -8972,7 +8993,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="170"/>
+      <c r="A57" s="185"/>
       <c r="B57" s="51" t="s">
         <v>59</v>
       </c>
@@ -8990,7 +9011,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="170"/>
+      <c r="A58" s="185"/>
       <c r="B58" s="51" t="s">
         <v>63</v>
       </c>
@@ -9008,7 +9029,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="170"/>
+      <c r="A59" s="185"/>
       <c r="B59" s="51" t="s">
         <v>55</v>
       </c>
@@ -9026,7 +9047,7 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="170"/>
+      <c r="A60" s="185"/>
       <c r="B60" s="51" t="s">
         <v>78</v>
       </c>
@@ -9044,7 +9065,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="171"/>
+      <c r="A61" s="186"/>
       <c r="B61" s="52" t="s">
         <v>263</v>
       </c>
@@ -9065,7 +9086,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="166" t="s">
+      <c r="A63" s="167" t="s">
         <v>270</v>
       </c>
       <c r="B63" s="67" t="s">
@@ -9084,7 +9105,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="167"/>
+      <c r="A64" s="168"/>
       <c r="B64" s="67" t="s">
         <v>54</v>
       </c>
@@ -9101,7 +9122,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="167"/>
+      <c r="A65" s="168"/>
       <c r="B65" s="67" t="s">
         <v>265</v>
       </c>
@@ -9118,7 +9139,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="167"/>
+      <c r="A66" s="168"/>
       <c r="B66" s="67" t="s">
         <v>266</v>
       </c>
@@ -9135,7 +9156,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="167"/>
+      <c r="A67" s="168"/>
       <c r="B67" s="67" t="s">
         <v>53</v>
       </c>
@@ -9152,7 +9173,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="167"/>
+      <c r="A68" s="168"/>
       <c r="B68" s="67" t="s">
         <v>63</v>
       </c>
@@ -9169,7 +9190,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="167"/>
+      <c r="A69" s="168"/>
       <c r="B69" s="67" t="s">
         <v>55</v>
       </c>
@@ -9186,7 +9207,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="167"/>
+      <c r="A70" s="168"/>
       <c r="B70" s="67" t="s">
         <v>267</v>
       </c>
@@ -9203,7 +9224,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="167"/>
+      <c r="A71" s="168"/>
       <c r="B71" s="67" t="s">
         <v>268</v>
       </c>
@@ -9220,7 +9241,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="167"/>
+      <c r="A72" s="168"/>
       <c r="B72" s="67" t="s">
         <v>269</v>
       </c>
@@ -9237,7 +9258,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="168"/>
+      <c r="A73" s="169"/>
       <c r="B73" s="68" t="s">
         <v>59</v>
       </c>
@@ -9258,7 +9279,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="196" t="s">
+      <c r="A75" s="179" t="s">
         <v>307</v>
       </c>
       <c r="B75" s="116" t="s">
@@ -9277,7 +9298,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="197"/>
+      <c r="A76" s="180"/>
       <c r="B76" s="119" t="s">
         <v>54</v>
       </c>
@@ -9294,7 +9315,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="197"/>
+      <c r="A77" s="180"/>
       <c r="B77" s="119" t="s">
         <v>312</v>
       </c>
@@ -9311,7 +9332,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="197"/>
+      <c r="A78" s="180"/>
       <c r="B78" s="119" t="s">
         <v>310</v>
       </c>
@@ -9328,7 +9349,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="197"/>
+      <c r="A79" s="180"/>
       <c r="B79" s="119" t="s">
         <v>53</v>
       </c>
@@ -9345,7 +9366,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="197"/>
+      <c r="A80" s="180"/>
       <c r="B80" s="119" t="s">
         <v>30</v>
       </c>
@@ -9362,7 +9383,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="197"/>
+      <c r="A81" s="180"/>
       <c r="B81" s="119" t="s">
         <v>55</v>
       </c>
@@ -9379,7 +9400,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="197"/>
+      <c r="A82" s="180"/>
       <c r="B82" s="119" t="s">
         <v>311</v>
       </c>
@@ -9396,7 +9417,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="197"/>
+      <c r="A83" s="180"/>
       <c r="B83" s="119" t="s">
         <v>63</v>
       </c>
@@ -9413,7 +9434,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="197"/>
+      <c r="A84" s="180"/>
       <c r="B84" s="119" t="s">
         <v>308</v>
       </c>
@@ -9430,7 +9451,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="197"/>
+      <c r="A85" s="180"/>
       <c r="B85" s="119" t="s">
         <v>306</v>
       </c>
@@ -9447,7 +9468,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="197"/>
+      <c r="A86" s="180"/>
       <c r="B86" s="119" t="s">
         <v>309</v>
       </c>
@@ -9464,7 +9485,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="198"/>
+      <c r="A87" s="181"/>
       <c r="B87" s="120" t="s">
         <v>59</v>
       </c>
@@ -9481,7 +9502,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="199" t="s">
+      <c r="A88" s="182" t="s">
         <v>315</v>
       </c>
       <c r="B88" s="122" t="s">
@@ -9500,7 +9521,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="200"/>
+      <c r="A89" s="183"/>
       <c r="B89" s="122" t="s">
         <v>313</v>
       </c>
@@ -9517,7 +9538,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="200"/>
+      <c r="A90" s="183"/>
       <c r="B90" s="122" t="s">
         <v>299</v>
       </c>
@@ -9534,7 +9555,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="200"/>
+      <c r="A91" s="183"/>
       <c r="B91" s="122" t="s">
         <v>30</v>
       </c>
@@ -9551,7 +9572,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="200"/>
+      <c r="A92" s="183"/>
       <c r="B92" s="122" t="s">
         <v>55</v>
       </c>
@@ -9568,7 +9589,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="200"/>
+      <c r="A93" s="183"/>
       <c r="B93" s="122" t="s">
         <v>75</v>
       </c>
@@ -9589,7 +9610,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="190" t="s">
+      <c r="A95" s="173" t="s">
         <v>316</v>
       </c>
       <c r="B95" s="128" t="s">
@@ -9608,7 +9629,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="191"/>
+      <c r="A96" s="174"/>
       <c r="B96" s="131" t="s">
         <v>53</v>
       </c>
@@ -9625,7 +9646,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="191"/>
+      <c r="A97" s="174"/>
       <c r="B97" s="131" t="s">
         <v>30</v>
       </c>
@@ -9642,7 +9663,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="191"/>
+      <c r="A98" s="174"/>
       <c r="B98" s="131" t="s">
         <v>55</v>
       </c>
@@ -9659,7 +9680,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="191"/>
+      <c r="A99" s="174"/>
       <c r="B99" s="131" t="s">
         <v>311</v>
       </c>
@@ -9676,7 +9697,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="191"/>
+      <c r="A100" s="174"/>
       <c r="B100" s="131" t="s">
         <v>63</v>
       </c>
@@ -9693,7 +9714,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="191"/>
+      <c r="A101" s="174"/>
       <c r="B101" s="131" t="s">
         <v>318</v>
       </c>
@@ -9710,7 +9731,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="191"/>
+      <c r="A102" s="174"/>
       <c r="B102" s="131" t="s">
         <v>319</v>
       </c>
@@ -9727,7 +9748,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="191"/>
+      <c r="A103" s="174"/>
       <c r="B103" s="131" t="s">
         <v>320</v>
       </c>
@@ -9744,7 +9765,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="191"/>
+      <c r="A104" s="174"/>
       <c r="B104" s="131" t="s">
         <v>308</v>
       </c>
@@ -9761,7 +9782,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="191"/>
+      <c r="A105" s="174"/>
       <c r="B105" s="131" t="s">
         <v>306</v>
       </c>
@@ -9778,7 +9799,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="191"/>
+      <c r="A106" s="174"/>
       <c r="B106" s="131" t="s">
         <v>317</v>
       </c>
@@ -9795,7 +9816,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="192"/>
+      <c r="A107" s="175"/>
       <c r="B107" s="132" t="s">
         <v>59</v>
       </c>
@@ -9816,7 +9837,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="193" t="s">
+      <c r="A109" s="176" t="s">
         <v>326</v>
       </c>
       <c r="B109" s="136" t="s">
@@ -9835,7 +9856,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="194"/>
+      <c r="A110" s="177"/>
       <c r="B110" s="139" t="s">
         <v>53</v>
       </c>
@@ -9852,7 +9873,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="194"/>
+      <c r="A111" s="177"/>
       <c r="B111" s="139" t="s">
         <v>54</v>
       </c>
@@ -9869,7 +9890,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="194"/>
+      <c r="A112" s="177"/>
       <c r="B112" s="139" t="s">
         <v>30</v>
       </c>
@@ -9886,7 +9907,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="194"/>
+      <c r="A113" s="177"/>
       <c r="B113" s="139" t="s">
         <v>55</v>
       </c>
@@ -9903,7 +9924,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="194"/>
+      <c r="A114" s="177"/>
       <c r="B114" s="139" t="s">
         <v>311</v>
       </c>
@@ -9920,7 +9941,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="194"/>
+      <c r="A115" s="177"/>
       <c r="B115" s="139" t="s">
         <v>63</v>
       </c>
@@ -9937,7 +9958,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="194"/>
+      <c r="A116" s="177"/>
       <c r="B116" s="139" t="s">
         <v>319</v>
       </c>
@@ -9954,7 +9975,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="194"/>
+      <c r="A117" s="177"/>
       <c r="B117" s="139" t="s">
         <v>320</v>
       </c>
@@ -9971,7 +9992,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="194"/>
+      <c r="A118" s="177"/>
       <c r="B118" s="139" t="s">
         <v>308</v>
       </c>
@@ -9988,7 +10009,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="194"/>
+      <c r="A119" s="177"/>
       <c r="B119" s="139" t="s">
         <v>80</v>
       </c>
@@ -10005,7 +10026,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="194"/>
+      <c r="A120" s="177"/>
       <c r="B120" s="139" t="s">
         <v>327</v>
       </c>
@@ -10022,7 +10043,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="194"/>
+      <c r="A121" s="177"/>
       <c r="B121" s="139" t="s">
         <v>328</v>
       </c>
@@ -10039,7 +10060,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="195"/>
+      <c r="A122" s="178"/>
       <c r="B122" s="140" t="s">
         <v>59</v>
       </c>
@@ -10056,7 +10077,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="187" t="s">
+      <c r="A123" s="170" t="s">
         <v>329</v>
       </c>
       <c r="B123" s="145" t="s">
@@ -10076,7 +10097,7 @@
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="188"/>
+      <c r="A124" s="171"/>
       <c r="B124" s="145" t="s">
         <v>289</v>
       </c>
@@ -10094,7 +10115,7 @@
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="188"/>
+      <c r="A125" s="171"/>
       <c r="B125" s="148" t="s">
         <v>330</v>
       </c>
@@ -10105,7 +10126,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="189"/>
+      <c r="A126" s="172"/>
       <c r="B126" s="145" t="s">
         <v>59</v>
       </c>
@@ -10128,11 +10149,6 @@
   </sheetData>
   <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="A109:A122"/>
-    <mergeCell ref="A75:A87"/>
-    <mergeCell ref="A88:A93"/>
     <mergeCell ref="A51:A61"/>
     <mergeCell ref="A63:A73"/>
     <mergeCell ref="A3:A13"/>
@@ -10140,6 +10156,11 @@
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A36:A42"/>
     <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="A109:A122"/>
+    <mergeCell ref="A75:A87"/>
+    <mergeCell ref="A88:A93"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added feeds to products
</commit_message>
<xml_diff>
--- a/lib/menu.xlsx
+++ b/lib/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Shadow Cakes App\webapp\shadowCakes\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D5A1E5-4D53-4323-8476-576500CACFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47BDBA6-B53E-4388-920D-09AD40639743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="926" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="361">
   <si>
     <t xml:space="preserve">vanilla </t>
   </si>
@@ -1175,6 +1175,13 @@
   </si>
   <si>
     <t>priceDiff</t>
+  </si>
+  <si>
+    <t>feeds</t>
+  </si>
+  <si>
+    <t>6 in feeds 5 people.
+8 in feeds 10 people.</t>
   </si>
 </sst>
 </file>
@@ -2256,6 +2263,60 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
@@ -2297,60 +2358,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="33" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="129">
@@ -2553,14 +2560,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2570,7 +2577,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2639,14 +2646,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2656,7 +2663,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2730,14 +2737,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2747,7 +2754,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3087,10 +3094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3409478-BB8A-4EB4-ACC6-5CDC2C1DB2F9}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3102,9 +3109,10 @@
     <col min="7" max="7" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.08203125" customWidth="1"/>
     <col min="13" max="13" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>350</v>
       </c>
@@ -3144,8 +3152,11 @@
       <c r="M1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -3185,8 +3196,11 @@
       <c r="M2" s="149" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="149" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="149" t="s">
         <v>336</v>
       </c>
@@ -3226,8 +3240,11 @@
       <c r="M3" s="149" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="149" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>339</v>
       </c>
@@ -3260,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="149" t="s">
         <v>341</v>
       </c>
@@ -3300,17 +3317,20 @@
       <c r="M5" s="149" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" s="149" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J6" s="149"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J7" s="149"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J8" s="149"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J9" s="149"/>
     </row>
   </sheetData>
@@ -8106,7 +8126,7 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="173" t="s">
         <v>239</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -8125,7 +8145,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="188"/>
+      <c r="A4" s="174"/>
       <c r="B4" s="11" t="s">
         <v>52</v>
       </c>
@@ -8142,7 +8162,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="188"/>
+      <c r="A5" s="174"/>
       <c r="B5" s="11" t="s">
         <v>64</v>
       </c>
@@ -8159,7 +8179,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="188"/>
+      <c r="A6" s="174"/>
       <c r="B6" s="11" t="s">
         <v>53</v>
       </c>
@@ -8176,7 +8196,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="188"/>
+      <c r="A7" s="174"/>
       <c r="B7" s="11" t="s">
         <v>54</v>
       </c>
@@ -8193,7 +8213,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="188"/>
+      <c r="A8" s="174"/>
       <c r="B8" s="11" t="s">
         <v>55</v>
       </c>
@@ -8210,7 +8230,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="188"/>
+      <c r="A9" s="174"/>
       <c r="B9" s="11" t="s">
         <v>56</v>
       </c>
@@ -8227,7 +8247,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="188"/>
+      <c r="A10" s="174"/>
       <c r="B10" s="11" t="s">
         <v>57</v>
       </c>
@@ -8244,7 +8264,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="188"/>
+      <c r="A11" s="174"/>
       <c r="B11" s="11" t="s">
         <v>68</v>
       </c>
@@ -8261,7 +8281,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="188"/>
+      <c r="A12" s="174"/>
       <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
@@ -8278,7 +8298,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="189"/>
+      <c r="A13" s="175"/>
       <c r="B13" s="11" t="s">
         <v>59</v>
       </c>
@@ -8299,7 +8319,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="190" t="s">
+      <c r="A15" s="176" t="s">
         <v>264</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -8318,7 +8338,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="191"/>
+      <c r="A16" s="177"/>
       <c r="B16" s="16" t="s">
         <v>52</v>
       </c>
@@ -8335,7 +8355,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="191"/>
+      <c r="A17" s="177"/>
       <c r="B17" s="16" t="s">
         <v>64</v>
       </c>
@@ -8352,7 +8372,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="191"/>
+      <c r="A18" s="177"/>
       <c r="B18" s="16" t="s">
         <v>53</v>
       </c>
@@ -8369,7 +8389,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="191"/>
+      <c r="A19" s="177"/>
       <c r="B19" s="16" t="s">
         <v>54</v>
       </c>
@@ -8386,7 +8406,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="191"/>
+      <c r="A20" s="177"/>
       <c r="B20" s="16" t="s">
         <v>55</v>
       </c>
@@ -8403,7 +8423,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="191"/>
+      <c r="A21" s="177"/>
       <c r="B21" s="16" t="s">
         <v>56</v>
       </c>
@@ -8420,7 +8440,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="191"/>
+      <c r="A22" s="177"/>
       <c r="B22" s="16" t="s">
         <v>57</v>
       </c>
@@ -8437,7 +8457,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="191"/>
+      <c r="A23" s="177"/>
       <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
@@ -8454,7 +8474,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="191"/>
+      <c r="A24" s="177"/>
       <c r="B24" s="16" t="s">
         <v>58</v>
       </c>
@@ -8471,7 +8491,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="191"/>
+      <c r="A25" s="177"/>
       <c r="B25" s="16" t="s">
         <v>59</v>
       </c>
@@ -8488,7 +8508,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="191"/>
+      <c r="A26" s="177"/>
       <c r="B26" s="16" t="s">
         <v>65</v>
       </c>
@@ -8506,7 +8526,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="192"/>
+      <c r="A27" s="178"/>
       <c r="B27" s="16" t="s">
         <v>66</v>
       </c>
@@ -8526,7 +8546,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="193" t="s">
+      <c r="A29" s="179" t="s">
         <v>245</v>
       </c>
       <c r="B29" s="51" t="s">
@@ -8546,7 +8566,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="194"/>
+      <c r="A30" s="180"/>
       <c r="B30" s="51" t="s">
         <v>246</v>
       </c>
@@ -8564,7 +8584,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="194"/>
+      <c r="A31" s="180"/>
       <c r="B31" s="51" t="s">
         <v>247</v>
       </c>
@@ -8582,7 +8602,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="194"/>
+      <c r="A32" s="180"/>
       <c r="B32" s="51" t="s">
         <v>56</v>
       </c>
@@ -8600,7 +8620,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="194"/>
+      <c r="A33" s="180"/>
       <c r="B33" s="51" t="s">
         <v>248</v>
       </c>
@@ -8618,7 +8638,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="195"/>
+      <c r="A34" s="181"/>
       <c r="B34" s="52" t="s">
         <v>249</v>
       </c>
@@ -8639,7 +8659,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="196" t="s">
+      <c r="A36" s="182" t="s">
         <v>253</v>
       </c>
       <c r="B36" s="56" t="s">
@@ -8659,7 +8679,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="197"/>
+      <c r="A37" s="183"/>
       <c r="B37" s="56" t="s">
         <v>246</v>
       </c>
@@ -8677,7 +8697,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="197"/>
+      <c r="A38" s="183"/>
       <c r="B38" s="56" t="s">
         <v>247</v>
       </c>
@@ -8695,7 +8715,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="197"/>
+      <c r="A39" s="183"/>
       <c r="B39" s="56" t="s">
         <v>56</v>
       </c>
@@ -8713,7 +8733,7 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="197"/>
+      <c r="A40" s="183"/>
       <c r="B40" s="56" t="s">
         <v>248</v>
       </c>
@@ -8731,7 +8751,7 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="197"/>
+      <c r="A41" s="183"/>
       <c r="B41" s="56" t="s">
         <v>252</v>
       </c>
@@ -8749,7 +8769,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="198"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="57" t="s">
         <v>249</v>
       </c>
@@ -8770,7 +8790,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="199" t="s">
+      <c r="A44" s="185" t="s">
         <v>255</v>
       </c>
       <c r="B44" s="64" t="s">
@@ -8790,7 +8810,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="200"/>
+      <c r="A45" s="186"/>
       <c r="B45" s="64" t="s">
         <v>246</v>
       </c>
@@ -8808,7 +8828,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="200"/>
+      <c r="A46" s="186"/>
       <c r="B46" s="64" t="s">
         <v>254</v>
       </c>
@@ -8826,7 +8846,7 @@
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="200"/>
+      <c r="A47" s="186"/>
       <c r="B47" s="64" t="s">
         <v>56</v>
       </c>
@@ -8844,7 +8864,7 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="200"/>
+      <c r="A48" s="186"/>
       <c r="B48" s="64" t="s">
         <v>248</v>
       </c>
@@ -8862,7 +8882,7 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="201"/>
+      <c r="A49" s="187"/>
       <c r="B49" s="26" t="s">
         <v>249</v>
       </c>
@@ -8883,7 +8903,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="184" t="s">
+      <c r="A51" s="170" t="s">
         <v>260</v>
       </c>
       <c r="B51" s="51" t="s">
@@ -8903,7 +8923,7 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="185"/>
+      <c r="A52" s="171"/>
       <c r="B52" s="51" t="s">
         <v>246</v>
       </c>
@@ -8921,7 +8941,7 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="185"/>
+      <c r="A53" s="171"/>
       <c r="B53" s="51" t="s">
         <v>262</v>
       </c>
@@ -8939,7 +8959,7 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="185"/>
+      <c r="A54" s="171"/>
       <c r="B54" s="51" t="s">
         <v>56</v>
       </c>
@@ -8957,7 +8977,7 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="185"/>
+      <c r="A55" s="171"/>
       <c r="B55" s="51" t="s">
         <v>75</v>
       </c>
@@ -8975,7 +8995,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="185"/>
+      <c r="A56" s="171"/>
       <c r="B56" s="51" t="s">
         <v>58</v>
       </c>
@@ -8993,7 +9013,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="185"/>
+      <c r="A57" s="171"/>
       <c r="B57" s="51" t="s">
         <v>59</v>
       </c>
@@ -9011,7 +9031,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="185"/>
+      <c r="A58" s="171"/>
       <c r="B58" s="51" t="s">
         <v>63</v>
       </c>
@@ -9029,7 +9049,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="185"/>
+      <c r="A59" s="171"/>
       <c r="B59" s="51" t="s">
         <v>55</v>
       </c>
@@ -9047,7 +9067,7 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="185"/>
+      <c r="A60" s="171"/>
       <c r="B60" s="51" t="s">
         <v>78</v>
       </c>
@@ -9065,7 +9085,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="186"/>
+      <c r="A61" s="172"/>
       <c r="B61" s="52" t="s">
         <v>263</v>
       </c>
@@ -9279,7 +9299,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="179" t="s">
+      <c r="A75" s="197" t="s">
         <v>307</v>
       </c>
       <c r="B75" s="116" t="s">
@@ -9298,7 +9318,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="180"/>
+      <c r="A76" s="198"/>
       <c r="B76" s="119" t="s">
         <v>54</v>
       </c>
@@ -9315,7 +9335,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="180"/>
+      <c r="A77" s="198"/>
       <c r="B77" s="119" t="s">
         <v>312</v>
       </c>
@@ -9332,7 +9352,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="180"/>
+      <c r="A78" s="198"/>
       <c r="B78" s="119" t="s">
         <v>310</v>
       </c>
@@ -9349,7 +9369,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="180"/>
+      <c r="A79" s="198"/>
       <c r="B79" s="119" t="s">
         <v>53</v>
       </c>
@@ -9366,7 +9386,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="180"/>
+      <c r="A80" s="198"/>
       <c r="B80" s="119" t="s">
         <v>30</v>
       </c>
@@ -9383,7 +9403,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="180"/>
+      <c r="A81" s="198"/>
       <c r="B81" s="119" t="s">
         <v>55</v>
       </c>
@@ -9400,7 +9420,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="180"/>
+      <c r="A82" s="198"/>
       <c r="B82" s="119" t="s">
         <v>311</v>
       </c>
@@ -9417,7 +9437,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="180"/>
+      <c r="A83" s="198"/>
       <c r="B83" s="119" t="s">
         <v>63</v>
       </c>
@@ -9434,7 +9454,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="180"/>
+      <c r="A84" s="198"/>
       <c r="B84" s="119" t="s">
         <v>308</v>
       </c>
@@ -9451,7 +9471,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="180"/>
+      <c r="A85" s="198"/>
       <c r="B85" s="119" t="s">
         <v>306</v>
       </c>
@@ -9468,7 +9488,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="180"/>
+      <c r="A86" s="198"/>
       <c r="B86" s="119" t="s">
         <v>309</v>
       </c>
@@ -9485,7 +9505,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="181"/>
+      <c r="A87" s="199"/>
       <c r="B87" s="120" t="s">
         <v>59</v>
       </c>
@@ -9502,7 +9522,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="182" t="s">
+      <c r="A88" s="200" t="s">
         <v>315</v>
       </c>
       <c r="B88" s="122" t="s">
@@ -9521,7 +9541,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="183"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="122" t="s">
         <v>313</v>
       </c>
@@ -9538,7 +9558,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="183"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="122" t="s">
         <v>299</v>
       </c>
@@ -9555,7 +9575,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="183"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="122" t="s">
         <v>30</v>
       </c>
@@ -9572,7 +9592,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="183"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="122" t="s">
         <v>55</v>
       </c>
@@ -9589,7 +9609,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="183"/>
+      <c r="A93" s="201"/>
       <c r="B93" s="122" t="s">
         <v>75</v>
       </c>
@@ -9610,7 +9630,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="173" t="s">
+      <c r="A95" s="191" t="s">
         <v>316</v>
       </c>
       <c r="B95" s="128" t="s">
@@ -9629,7 +9649,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="174"/>
+      <c r="A96" s="192"/>
       <c r="B96" s="131" t="s">
         <v>53</v>
       </c>
@@ -9646,7 +9666,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="174"/>
+      <c r="A97" s="192"/>
       <c r="B97" s="131" t="s">
         <v>30</v>
       </c>
@@ -9663,7 +9683,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="174"/>
+      <c r="A98" s="192"/>
       <c r="B98" s="131" t="s">
         <v>55</v>
       </c>
@@ -9680,7 +9700,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="174"/>
+      <c r="A99" s="192"/>
       <c r="B99" s="131" t="s">
         <v>311</v>
       </c>
@@ -9697,7 +9717,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="174"/>
+      <c r="A100" s="192"/>
       <c r="B100" s="131" t="s">
         <v>63</v>
       </c>
@@ -9714,7 +9734,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="174"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="131" t="s">
         <v>318</v>
       </c>
@@ -9731,7 +9751,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="174"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="131" t="s">
         <v>319</v>
       </c>
@@ -9748,7 +9768,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="174"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="131" t="s">
         <v>320</v>
       </c>
@@ -9765,7 +9785,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="174"/>
+      <c r="A104" s="192"/>
       <c r="B104" s="131" t="s">
         <v>308</v>
       </c>
@@ -9782,7 +9802,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="174"/>
+      <c r="A105" s="192"/>
       <c r="B105" s="131" t="s">
         <v>306</v>
       </c>
@@ -9799,7 +9819,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="174"/>
+      <c r="A106" s="192"/>
       <c r="B106" s="131" t="s">
         <v>317</v>
       </c>
@@ -9816,7 +9836,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="175"/>
+      <c r="A107" s="193"/>
       <c r="B107" s="132" t="s">
         <v>59</v>
       </c>
@@ -9837,7 +9857,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="176" t="s">
+      <c r="A109" s="194" t="s">
         <v>326</v>
       </c>
       <c r="B109" s="136" t="s">
@@ -9856,7 +9876,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="177"/>
+      <c r="A110" s="195"/>
       <c r="B110" s="139" t="s">
         <v>53</v>
       </c>
@@ -9873,7 +9893,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="177"/>
+      <c r="A111" s="195"/>
       <c r="B111" s="139" t="s">
         <v>54</v>
       </c>
@@ -9890,7 +9910,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="177"/>
+      <c r="A112" s="195"/>
       <c r="B112" s="139" t="s">
         <v>30</v>
       </c>
@@ -9907,7 +9927,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="177"/>
+      <c r="A113" s="195"/>
       <c r="B113" s="139" t="s">
         <v>55</v>
       </c>
@@ -9924,7 +9944,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="177"/>
+      <c r="A114" s="195"/>
       <c r="B114" s="139" t="s">
         <v>311</v>
       </c>
@@ -9941,7 +9961,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="177"/>
+      <c r="A115" s="195"/>
       <c r="B115" s="139" t="s">
         <v>63</v>
       </c>
@@ -9958,7 +9978,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="177"/>
+      <c r="A116" s="195"/>
       <c r="B116" s="139" t="s">
         <v>319</v>
       </c>
@@ -9975,7 +9995,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="177"/>
+      <c r="A117" s="195"/>
       <c r="B117" s="139" t="s">
         <v>320</v>
       </c>
@@ -9992,7 +10012,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="177"/>
+      <c r="A118" s="195"/>
       <c r="B118" s="139" t="s">
         <v>308</v>
       </c>
@@ -10009,7 +10029,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="177"/>
+      <c r="A119" s="195"/>
       <c r="B119" s="139" t="s">
         <v>80</v>
       </c>
@@ -10026,7 +10046,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="177"/>
+      <c r="A120" s="195"/>
       <c r="B120" s="139" t="s">
         <v>327</v>
       </c>
@@ -10043,7 +10063,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="177"/>
+      <c r="A121" s="195"/>
       <c r="B121" s="139" t="s">
         <v>328</v>
       </c>
@@ -10060,7 +10080,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="178"/>
+      <c r="A122" s="196"/>
       <c r="B122" s="140" t="s">
         <v>59</v>
       </c>
@@ -10077,7 +10097,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="170" t="s">
+      <c r="A123" s="188" t="s">
         <v>329</v>
       </c>
       <c r="B123" s="145" t="s">
@@ -10097,7 +10117,7 @@
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="171"/>
+      <c r="A124" s="189"/>
       <c r="B124" s="145" t="s">
         <v>289</v>
       </c>
@@ -10115,7 +10135,7 @@
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="171"/>
+      <c r="A125" s="189"/>
       <c r="B125" s="148" t="s">
         <v>330</v>
       </c>
@@ -10126,7 +10146,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="172"/>
+      <c r="A126" s="190"/>
       <c r="B126" s="145" t="s">
         <v>59</v>
       </c>
@@ -10149,6 +10169,11 @@
   </sheetData>
   <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="A109:A122"/>
+    <mergeCell ref="A75:A87"/>
+    <mergeCell ref="A88:A93"/>
     <mergeCell ref="A51:A61"/>
     <mergeCell ref="A63:A73"/>
     <mergeCell ref="A3:A13"/>
@@ -10156,11 +10181,6 @@
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A36:A42"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="A109:A122"/>
-    <mergeCell ref="A75:A87"/>
-    <mergeCell ref="A88:A93"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>